<commit_message>
commiting changes of host transaction report
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/OCMIvrHostTransactionReport.xlsx
+++ b/ocms/src/test/resources/TestData/OCMIvrHostTransactionReport.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD9B2B9-8EC9-4739-93F3-7E65B5D340EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564545AF-8AB5-4B57-9CAE-7D38E83BB0D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="50">
   <si>
     <t>Report Channel</t>
   </si>
@@ -107,12 +107,27 @@
     <t>Deleted</t>
   </si>
   <si>
+    <t>17-06-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>19-06-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>10000002001592375975</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
     <t>User ID</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
+    <t>18-06-2020 00:00:00</t>
+  </si>
+  <si>
     <t>Report Name1</t>
   </si>
   <si>
@@ -120,6 +135,9 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>15-06-2020 00:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">SELECT [UCID],FORMAT([dbo].[VARCHARTODATETIME] (REQUESTDATETIME),'dd/MM/yyyy HH:mm:ss') as [Request Date Time],[CIN] as [CIN/NRIC],
@@ -141,47 +159,44 @@
     <t>N</t>
   </si>
   <si>
+    <t>10000002051592461233</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>15-01-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>15-04-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>17-03-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>10000001881615967106</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>10000001891615967165</t>
-  </si>
-  <si>
-    <t>01-01-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>29-04-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>14-04-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>18-03-2021 00:00:00</t>
+    <t>Menu Description</t>
+  </si>
+  <si>
+    <t>Is not equal to</t>
+  </si>
+  <si>
+    <t>OTP_GEN</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>Does not contain</t>
+  </si>
+  <si>
+    <t>CIF</t>
+  </si>
+  <si>
+    <t>Starts with</t>
+  </si>
+  <si>
+    <t>Ends with</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,19 +209,19 @@
       <color rgb="FF444444"/>
       <name val="OCMFont"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -238,6 +253,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +545,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -551,13 +575,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -571,7 +595,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -621,7 +645,7 @@
         <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -629,16 +653,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>35</v>
+      <c r="D2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>19</v>
@@ -650,13 +674,13 @@
         <v>16</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -664,16 +688,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>35</v>
+      <c r="D3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>19</v>
@@ -685,7 +709,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="J3" s="8"/>
     </row>
@@ -694,16 +718,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>35</v>
+      <c r="D4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>19</v>
@@ -715,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J4" s="8"/>
     </row>
@@ -724,28 +748,28 @@
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>35</v>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J5" s="8"/>
     </row>
@@ -754,28 +778,28 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>35</v>
+      <c r="D6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J6" s="8"/>
     </row>
@@ -784,16 +808,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
+      <c r="D7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>19</v>
@@ -805,12 +829,11 @@
         <v>16</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -821,7 +844,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -851,13 +874,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -870,7 +893,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -903,16 +926,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>35</v>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +948,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -951,7 +974,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -959,16 +982,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -980,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1011,7 +1034,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>18</v>
@@ -1022,19 +1045,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>44</v>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>25</v>
@@ -1047,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1068,37 +1091,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1107,16 +1130,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>35</v>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -1128,14 +1151,161 @@
         <v>16</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1177,7 +1347,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.5">
@@ -1185,19 +1355,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>